<commit_message>
Corrections to 4-Word-Memory-Clear program supporting files.
</commit_message>
<xml_diff>
--- a/4-Word-Memory-Clear/4-Word-Memory-Clear-Timing.xlsx
+++ b/4-Word-Memory-Clear/4-Word-Memory-Clear-Timing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paulk\Documents\Projects\Bendix-G-15\G15-software\4-Word-Memory-Clear\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACE6D75-BF4B-4FD7-8898-351205AFC9AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681645B8-45E5-42FE-8950-1B2C622DFAB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1470" yWindow="480" windowWidth="16680" windowHeight="15720" xr2:uid="{575D24E0-B257-4811-8BEE-8643A635021B}"/>
   </bookViews>
@@ -113,7 +113,7 @@
     <t>Clear Cycle Timing, word-times</t>
   </si>
   <si>
-    <t>2025-07-08</t>
+    <t>2025-07-09</t>
   </si>
 </sst>
 </file>
@@ -172,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -183,10 +183,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -527,7 +532,9 @@
   </sheetPr>
   <dimension ref="A1:W22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -535,13 +542,15 @@
     <col min="9" max="15" width="5" customWidth="1"/>
     <col min="16" max="16" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="3.7109375" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="V1" s="2"/>
+      <c r="W1" s="7" t="s">
         <v>25</v>
       </c>
     </row>
@@ -902,11 +911,11 @@
       </c>
       <c r="S9" s="5"/>
       <c r="T9" s="5"/>
-      <c r="U9" s="7">
+      <c r="U9" s="6">
         <f>SUM(U4:U8)</f>
         <v>324</v>
       </c>
-      <c r="V9" s="6" t="s">
+      <c r="V9" s="9" t="s">
         <v>21</v>
       </c>
       <c r="W9" s="1">
@@ -1095,7 +1104,7 @@
         <v>20</v>
       </c>
       <c r="U17">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
@@ -1281,16 +1290,16 @@
       </c>
       <c r="S21" s="5"/>
       <c r="T21" s="5"/>
-      <c r="U21" s="7">
+      <c r="U21" s="6">
         <f>SUM(U16:U20)</f>
-        <v>647</v>
-      </c>
-      <c r="V21" s="6" t="s">
+        <v>648</v>
+      </c>
+      <c r="V21" s="9" t="s">
         <v>21</v>
       </c>
       <c r="W21" s="1">
         <f>U21*30</f>
-        <v>19410</v>
+        <v>19440</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>